<commit_message>
Versão 4 = Consegue fazer o download da guia itens e anexo ( concomitantemente )
</commit_message>
<xml_diff>
--- a/dados/Teste.xlsx
+++ b/dados/Teste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Requisição</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Status da RequisiÃ§Ã£o</t>
-  </si>
-  <si>
-    <t>RequisiÃ§Ã£o Consumo de Contrato</t>
   </si>
   <si>
     <t>Aprovado</t>
@@ -368,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +378,7 @@
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,32 +389,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8167172</v>
+        <v>8167085</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8167085</v>
+        <v>8166505</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1">
-        <v>8167116</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8167172</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -429,6 +424,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AD8D136BA8CE0949B36B2F8738B888E9" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c2f93e0e6fd10c7cb521d7cd6f006c3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df034896-8502-4d67-9cfb-48e355cdb79d" xmlns:ns4="68ed8c79-16b4-498b-bef1-d9e3f554bf12" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="312d5512dd76f8ae45b4d5f1c1fa245e" ns3:_="" ns4:_="">
     <xsd:import namespace="df034896-8502-4d67-9cfb-48e355cdb79d"/>
@@ -637,15 +641,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -653,6 +648,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE6A8B5-869C-4F06-BA69-8CF6BC9A8FE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191E0179-7B80-4D4B-8141-31B2FA29717E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -671,27 +674,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE6A8B5-869C-4F06-BA69-8CF6BC9A8FE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8794E490-A007-4E7F-8686-04A3292010BA}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="df034896-8502-4d67-9cfb-48e355cdb79d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="68ed8c79-16b4-498b-bef1-d9e3f554bf12"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="68ed8c79-16b4-498b-bef1-d9e3f554bf12"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>